<commit_message>
Updated Girish Data Model
</commit_message>
<xml_diff>
--- a/Team Members Work/Girishkumar/Girish- Data Model.xlsx
+++ b/Team Members Work/Girishkumar/Girish- Data Model.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FA1BEB2-A056-4534-BCAB-7CBB8C6754E6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7D95E54-BF81-41C2-AF2C-1701280E6B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>User</t>
   </si>
@@ -107,15 +107,33 @@
     <t>Ambika</t>
   </si>
   <si>
+    <t>TravelDetails</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
     <t>TrainDetails</t>
   </si>
   <si>
-    <t>Payment</t>
+    <t>TravelID</t>
   </si>
   <si>
     <t>TrainNo</t>
   </si>
   <si>
+    <t>ClassId</t>
+  </si>
+  <si>
+    <t>QuotaId</t>
+  </si>
+  <si>
+    <t>PaymentGateway</t>
+  </si>
+  <si>
+    <t>PaymentId</t>
+  </si>
+  <si>
     <t>TrainName</t>
   </si>
   <si>
@@ -128,16 +146,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>ClassId</t>
-  </si>
-  <si>
-    <t>QuotaId</t>
-  </si>
-  <si>
-    <t>PaymentGateway</t>
-  </si>
-  <si>
-    <t>PaymentId</t>
+    <t>Gpay</t>
   </si>
   <si>
     <t>Kovai express</t>
@@ -150,9 +159,6 @@
   </si>
   <si>
     <t>15.04.22</t>
-  </si>
-  <si>
-    <t>Gpay</t>
   </si>
   <si>
     <t>keralaexpress</t>
@@ -254,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +270,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,10 +293,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -600,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="Y42" sqref="Y42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -612,7 +625,7 @@
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:21">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -655,7 +668,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:21">
       <c r="A3">
         <v>1</v>
       </c>
@@ -690,7 +703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:21">
       <c r="A4">
         <v>2</v>
       </c>
@@ -725,7 +738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:21">
       <c r="A5">
         <v>3</v>
       </c>
@@ -760,73 +773,73 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="C8" s="1" t="s">
+    <row r="8" spans="1:21">
+      <c r="E8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" t="s">
+      <c r="S8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="9" spans="1:21">
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" t="s">
+      <c r="J9" t="s">
         <v>33</v>
       </c>
-      <c r="G9" t="s">
+      <c r="K9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" t="s">
         <v>34</v>
       </c>
-      <c r="J9" t="s">
+      <c r="Q9" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" t="s">
         <v>35</v>
       </c>
-      <c r="K9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="S9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10">
+      <c r="T9" t="s">
+        <v>37</v>
+      </c>
+      <c r="U9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>4567</v>
       </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
         <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="J10" t="s">
-        <v>41</v>
       </c>
       <c r="K10">
         <v>8987</v>
@@ -837,31 +850,37 @@
       <c r="M10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11">
+      <c r="Q10">
+        <v>4567</v>
+      </c>
+      <c r="R10" t="s">
+        <v>40</v>
+      </c>
+      <c r="S10" t="s">
+        <v>41</v>
+      </c>
+      <c r="T10" t="s">
+        <v>42</v>
+      </c>
+      <c r="U10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
         <v>8987</v>
       </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
+      <c r="E11">
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K11">
         <v>8987</v>
@@ -872,31 +891,37 @@
       <c r="M11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12">
+      <c r="Q11">
+        <v>8987</v>
+      </c>
+      <c r="R11" t="s">
+        <v>44</v>
+      </c>
+      <c r="S11" t="s">
+        <v>41</v>
+      </c>
+      <c r="T11" t="s">
+        <v>17</v>
+      </c>
+      <c r="U11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
         <v>9897</v>
       </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
+      <c r="E12">
+        <v>2</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
       <c r="J12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K12">
         <v>8987</v>
@@ -907,38 +932,53 @@
       <c r="M12">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="Q12">
+        <v>9897</v>
+      </c>
+      <c r="R12" t="s">
+        <v>46</v>
+      </c>
+      <c r="S12" t="s">
+        <v>41</v>
+      </c>
+      <c r="T12" t="s">
+        <v>47</v>
+      </c>
+      <c r="U12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>500</v>
@@ -947,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -955,7 +995,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D17">
         <v>800</v>
@@ -964,7 +1004,7 @@
         <v>2</v>
       </c>
       <c r="L17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -972,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D18">
         <v>900</v>
@@ -981,15 +1021,15 @@
         <v>3</v>
       </c>
       <c r="L18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="2:13">
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="2:13">
@@ -997,16 +1037,16 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M21" t="s">
         <v>2</v>
@@ -1017,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J22">
         <v>8787</v>
@@ -1037,7 +1077,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J23">
         <v>9898</v>
@@ -1057,7 +1097,7 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J24">
         <v>7878</v>
@@ -1074,7 +1114,7 @@
     </row>
     <row r="26" spans="2:13">
       <c r="H26" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -1082,19 +1122,19 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H27" t="s">
         <v>7</v>
       </c>
       <c r="I27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J27" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="2:13">

</xml_diff>